<commit_message>
Updated issue list file
Updated new feature part.
</commit_message>
<xml_diff>
--- a/Issue List/IssueChatAppAjax.xlsx
+++ b/Issue List/IssueChatAppAjax.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>Issue Number</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Validation part not done</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -482,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,10 +669,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +683,7 @@
     <col min="4" max="4" width="63.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -693,8 +696,11 @@
       <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>201</v>
       </c>
@@ -708,7 +714,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>202</v>
       </c>
@@ -722,7 +728,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>203</v>
       </c>
@@ -736,7 +742,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>204</v>
       </c>
@@ -748,6 +754,9 @@
       </c>
       <c r="D6" t="s">
         <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>